<commit_message>
Multiple Bundle alpha review
Started to review how alpha is calculated and effect of exit temperature
on alpha values
</commit_message>
<xml_diff>
--- a/Generic C9 HTS Data.xlsx
+++ b/Generic C9 HTS Data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Izaak\Documents\Research\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Izaak-PC\Documents\Research\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -3362,10 +3362,15 @@
   <dimension ref="A1:N40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="27" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">

</xml_diff>